<commit_message>
Edit định dạng ngày tháng import excel sinhvien
</commit_message>
<xml_diff>
--- a/WebApplication1/Content/testsv.xlsx
+++ b/WebApplication1/Content/testsv.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>MSSV</t>
   </si>
@@ -65,6 +65,15 @@
     <t>gioitinh</t>
   </si>
   <si>
+    <t>D14-TH01</t>
+  </si>
+  <si>
+    <t>K001</t>
+  </si>
+  <si>
+    <t>Ngay sinh</t>
+  </si>
+  <si>
     <t>DH51400074</t>
   </si>
   <si>
@@ -74,22 +83,7 @@
     <t>26 Quách Đình Bảo, P.Phú Thạnh, Q.Tân Phú</t>
   </si>
   <si>
-    <t>0902323980</t>
-  </si>
-  <si>
     <t>dieutrieuphieu96@gmail.com</t>
-  </si>
-  <si>
-    <t>D14-TH01</t>
-  </si>
-  <si>
-    <t>K001</t>
-  </si>
-  <si>
-    <t>Ngay sinh</t>
-  </si>
-  <si>
-    <t>15/12/1996</t>
   </si>
 </sst>
 </file>
@@ -206,17 +200,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,7 +494,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -509,12 +503,12 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10"/>
+      <c r="C1" s="12"/>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -538,43 +532,42 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10">
+        <v>35065</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>902323980</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="8" t="b">
+      <c r="K2" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>